<commit_message>
ch8-diagrams.xlsx: added data shape info
</commit_message>
<xml_diff>
--- a/ml/tf/tf-from-scratch/3/code-exercises/ch8/ch8-diagrams.xlsx
+++ b/ml/tf/tf-from-scratch/3/code-exercises/ch8/ch8-diagrams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\codelab\gpu\ml\tf\tf-from-scratch\3\code-exercises\ch8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD29900-12C7-4C93-8879-FB5BA5F2F61E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC632226-EE9D-4A78-86E8-7018B9A99110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="12504" xr2:uid="{11A5D9EC-664C-4C65-B657-EC97B5A44BD7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{11A5D9EC-664C-4C65-B657-EC97B5A44BD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>rnn cell</t>
   </si>
@@ -79,13 +79,40 @@
   </si>
   <si>
     <t>sum</t>
+  </si>
+  <si>
+    <t>data generated</t>
+  </si>
+  <si>
+    <t>254, 4, 2</t>
+  </si>
+  <si>
+    <t>254=samples</t>
+  </si>
+  <si>
+    <t>4=corners</t>
+  </si>
+  <si>
+    <t>2=directions</t>
+  </si>
+  <si>
+    <t>forward</t>
+  </si>
+  <si>
+    <t>input:</t>
+  </si>
+  <si>
+    <t>X[0:1]=[2,2]</t>
+  </si>
+  <si>
+    <t>X=[4,2] 1st of 254</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +122,14 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -151,13 +186,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -852,24 +887,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2FCD38F-A89D-4CAD-83E5-E3FBC2822CB9}">
-  <dimension ref="C5:H13"/>
+  <dimension ref="C5:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="18.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="18.36328125" style="1"/>
+    <col min="1" max="16384" width="18.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="D5" s="6" t="s">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="3:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="3:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
@@ -877,16 +912,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F7" s="4"/>
       <c r="G7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
@@ -896,7 +930,7 @@
       <c r="E8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -906,19 +940,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="4"/>
       <c r="G9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.35">
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="3" t="s">
         <v>3</v>
       </c>
@@ -928,16 +958,52 @@
       <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D12" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="D13" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D21" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>